<commit_message>
New signatures from the freshly splitted signature sheet
</commit_message>
<xml_diff>
--- a/uli-signed.xlsx
+++ b/uli-signed.xlsx
@@ -848,16 +848,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>29880</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>386280</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>266040</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>811800</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>48240</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>192600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,8 +870,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5417640" y="6772680"/>
-          <a:ext cx="1750320" cy="584640"/>
+          <a:off x="5229720" y="6641280"/>
+          <a:ext cx="2516400" cy="820080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -895,10 +895,10 @@
   <dimension ref="A1:BL52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8"/>
@@ -911,7 +911,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="6.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="15" style="1" width="9.13"/>
   </cols>
   <sheetData>

</xml_diff>